<commit_message>
Update entire Excel_analysis folder
</commit_message>
<xml_diff>
--- a/Derrick_Lux_Excel.xlsx
+++ b/Derrick_Lux_Excel.xlsx
@@ -1191,6 +1191,27 @@
   </cellStyles>
   <dxfs count="52">
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.00000000"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
@@ -1203,22 +1224,22 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.000000"/>
+      <numFmt numFmtId="168" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="0.0000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000000"/>
+      <numFmt numFmtId="170" formatCode="0.00000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1236,13 +1257,13 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -1270,27 +1291,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1653,7 +1653,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1898,7 +1897,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2019,7 +2017,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2094,7 +2091,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4401,7 +4397,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4451,7 +4446,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -4489,9 +4483,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -4871,9 +4863,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5281,7 +5271,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5412,7 +5401,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5661,7 +5649,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5792,7 +5779,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6197,7 +6183,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6318,7 +6303,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6393,7 +6377,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6524,7 +6507,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6769,7 +6751,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6890,7 +6871,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6965,7 +6945,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7096,7 +7075,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7341,7 +7319,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7462,7 +7439,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7537,7 +7513,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19644,924 +19619,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18">
-  <location ref="A8:D12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Average of Ratings" fld="6" subtotal="average" baseField="8" baseItem="0" numFmtId="164"/>
-    <dataField name="Sum of Discount" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="Count of Review" fld="5" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="10">
-    <format dxfId="9">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="8">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="7">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="3">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="2">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="30">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="28" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="29">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="30">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="31">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="32" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="33">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="34">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="35">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
-  <location ref="A39:C43" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Current price" fld="1" baseField="8" baseItem="0"/>
-    <dataField name="Sum of old price" fld="2" baseField="8" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A31:C35" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="104">
-        <item x="19"/>
-        <item x="86"/>
-        <item x="102"/>
-        <item x="35"/>
-        <item x="78"/>
-        <item x="29"/>
-        <item x="16"/>
-        <item x="97"/>
-        <item x="47"/>
-        <item x="72"/>
-        <item x="40"/>
-        <item x="90"/>
-        <item x="80"/>
-        <item x="48"/>
-        <item x="59"/>
-        <item x="77"/>
-        <item x="15"/>
-        <item x="65"/>
-        <item x="63"/>
-        <item x="36"/>
-        <item x="54"/>
-        <item x="24"/>
-        <item x="58"/>
-        <item x="101"/>
-        <item x="56"/>
-        <item x="39"/>
-        <item x="51"/>
-        <item x="13"/>
-        <item x="66"/>
-        <item x="92"/>
-        <item x="1"/>
-        <item x="12"/>
-        <item x="41"/>
-        <item x="83"/>
-        <item x="81"/>
-        <item x="45"/>
-        <item x="70"/>
-        <item x="52"/>
-        <item x="69"/>
-        <item x="10"/>
-        <item x="84"/>
-        <item x="21"/>
-        <item x="87"/>
-        <item x="0"/>
-        <item x="67"/>
-        <item x="74"/>
-        <item x="30"/>
-        <item x="7"/>
-        <item x="11"/>
-        <item x="18"/>
-        <item x="43"/>
-        <item x="61"/>
-        <item x="93"/>
-        <item x="98"/>
-        <item x="73"/>
-        <item x="44"/>
-        <item x="46"/>
-        <item x="60"/>
-        <item x="8"/>
-        <item x="85"/>
-        <item x="26"/>
-        <item x="95"/>
-        <item x="50"/>
-        <item x="75"/>
-        <item x="89"/>
-        <item x="79"/>
-        <item x="82"/>
-        <item x="88"/>
-        <item x="68"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="34"/>
-        <item x="22"/>
-        <item x="99"/>
-        <item x="49"/>
-        <item x="76"/>
-        <item x="14"/>
-        <item x="71"/>
-        <item x="4"/>
-        <item x="27"/>
-        <item x="100"/>
-        <item x="31"/>
-        <item x="20"/>
-        <item x="96"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="17"/>
-        <item x="23"/>
-        <item x="57"/>
-        <item x="42"/>
-        <item x="55"/>
-        <item x="2"/>
-        <item x="28"/>
-        <item x="64"/>
-        <item x="6"/>
-        <item x="38"/>
-        <item x="53"/>
-        <item x="25"/>
-        <item x="5"/>
-        <item x="91"/>
-        <item x="94"/>
-        <item x="62"/>
-        <item x="37"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Average of Current price" fld="1" subtotal="average" baseField="7" baseItem="0"/>
-    <dataField name="Average of old price" fld="2" subtotal="average" baseField="7" baseItem="0"/>
-  </dataFields>
-  <formats count="8">
-    <format dxfId="17">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="16">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="15">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="14">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="12">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="11">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="10">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Count of Ratings" fld="6" subtotal="count" baseField="0" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Discount" fld="3" subtotal="average" baseField="7" baseItem="1"/>
-  </dataFields>
-  <formats count="9">
-    <format dxfId="26">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="7" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="24">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="23">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="22">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="21">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="20">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="19">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="18">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
   <location ref="A15:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
@@ -21008,25 +20065,25 @@
     <dataField name="Average of Ratings" fld="6" subtotal="average" baseField="7" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="33">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -21063,6 +20120,924 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18">
+  <location ref="A8:D12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Average of Ratings" fld="6" subtotal="average" baseField="8" baseItem="0" numFmtId="164"/>
+    <dataField name="Sum of Discount" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Count of Review" fld="5" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="10">
+    <format dxfId="16">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="30">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="28" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="29">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="30">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="31">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="32" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="33">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="34">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="35">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+  <location ref="A39:C43" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Current price" fld="1" baseField="8" baseItem="0"/>
+    <dataField name="Sum of old price" fld="2" baseField="8" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A31:C35" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="104">
+        <item x="19"/>
+        <item x="86"/>
+        <item x="102"/>
+        <item x="35"/>
+        <item x="78"/>
+        <item x="29"/>
+        <item x="16"/>
+        <item x="97"/>
+        <item x="47"/>
+        <item x="72"/>
+        <item x="40"/>
+        <item x="90"/>
+        <item x="80"/>
+        <item x="48"/>
+        <item x="59"/>
+        <item x="77"/>
+        <item x="15"/>
+        <item x="65"/>
+        <item x="63"/>
+        <item x="36"/>
+        <item x="54"/>
+        <item x="24"/>
+        <item x="58"/>
+        <item x="101"/>
+        <item x="56"/>
+        <item x="39"/>
+        <item x="51"/>
+        <item x="13"/>
+        <item x="66"/>
+        <item x="92"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="41"/>
+        <item x="83"/>
+        <item x="81"/>
+        <item x="45"/>
+        <item x="70"/>
+        <item x="52"/>
+        <item x="69"/>
+        <item x="10"/>
+        <item x="84"/>
+        <item x="21"/>
+        <item x="87"/>
+        <item x="0"/>
+        <item x="67"/>
+        <item x="74"/>
+        <item x="30"/>
+        <item x="7"/>
+        <item x="11"/>
+        <item x="18"/>
+        <item x="43"/>
+        <item x="61"/>
+        <item x="93"/>
+        <item x="98"/>
+        <item x="73"/>
+        <item x="44"/>
+        <item x="46"/>
+        <item x="60"/>
+        <item x="8"/>
+        <item x="85"/>
+        <item x="26"/>
+        <item x="95"/>
+        <item x="50"/>
+        <item x="75"/>
+        <item x="89"/>
+        <item x="79"/>
+        <item x="82"/>
+        <item x="88"/>
+        <item x="68"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="34"/>
+        <item x="22"/>
+        <item x="99"/>
+        <item x="49"/>
+        <item x="76"/>
+        <item x="14"/>
+        <item x="71"/>
+        <item x="4"/>
+        <item x="27"/>
+        <item x="100"/>
+        <item x="31"/>
+        <item x="20"/>
+        <item x="96"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="17"/>
+        <item x="23"/>
+        <item x="57"/>
+        <item x="42"/>
+        <item x="55"/>
+        <item x="2"/>
+        <item x="28"/>
+        <item x="64"/>
+        <item x="6"/>
+        <item x="38"/>
+        <item x="53"/>
+        <item x="25"/>
+        <item x="5"/>
+        <item x="91"/>
+        <item x="94"/>
+        <item x="62"/>
+        <item x="37"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Average of Current price" fld="1" subtotal="average" baseField="7" baseItem="0"/>
+    <dataField name="Average of old price" fld="2" subtotal="average" baseField="7" baseItem="0"/>
+  </dataFields>
+  <formats count="8">
+    <format dxfId="24">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="23">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="21">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="20">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="17">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Ratings" fld="6" subtotal="count" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Discount" fld="3" subtotal="average" baseField="7" baseItem="1"/>
+  </dataFields>
+  <formats count="9">
+    <format dxfId="33">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="7" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="31">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="29">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="28">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="27">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="25">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>

</xml_diff>